<commit_message>
Pushing the release_note into the branch: release/8.0.0
</commit_message>
<xml_diff>
--- a/helm-charts/uat-values/release_note/release-note-summary.xlsx
+++ b/helm-charts/uat-values/release_note/release-note-summary.xlsx
@@ -693,7 +693,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>"AQST"</t>
+          <t>AQST</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -787,7 +787,7 @@
     "image": {
         "imageName": "asia-south1-docker.pkg.dev/nice-virtue-463917-m0/service-admin/admin:14-uat",
         "pullPolicy": "IfNotPresent",
-        "repouatory": "asia-south1-docker.pkg.dev/nice-virtue-463917-m0/service-admin/admin",
+        "repository": "asia-south1-docker.pkg.dev/nice-virtue-463917-m0/service-admin/admin",
         "tag": "12-uat"
     },
     "replicaCount": 1,
@@ -900,7 +900,7 @@
     "image": {
         "imageName": "asia-south1-docker.pkg.dev/nice-virtue-463917-m0/service-auth/auth:12-uat",
         "pullPolicy": "IfNotPresent",
-        "repouatory": "asia-south1-docker.pkg.dev/nice-virtue-463917-m0/service-auth/auth",
+        "repository": "asia-south1-docker.pkg.dev/nice-virtue-463917-m0/service-auth/auth",
         "tag": "12-uat"
     },
     "replicaCount": 1,
@@ -1013,7 +1013,7 @@
     "image": {
         "imageName": "asia-south1-docker.pkg.dev/nice-virtue-463917-m0/service-user/user:48-uat",
         "pullPolicy": "IfNotPresent",
-        "repouatory": "asia-south1-docker.pkg.dev/nice-virtue-463917-m0/service-user/user",
+        "repository": "asia-south1-docker.pkg.dev/nice-virtue-463917-m0/service-user/user",
         "tag": "48-uat"
     },
     "replicaCount": 1,

</xml_diff>